<commit_message>
Checked numbers for figure 5 & 6 and fixed up character strinsg for a couple figures
</commit_message>
<xml_diff>
--- a/Data/Pmystaceus_trials_summary.xlsx
+++ b/Data/Pmystaceus_trials_summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinwhiting/Dropbox/Phrynocephalus_mystaceus/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielnoble/Dropbox/1_Research/1_Manuscripts/In_Preparation/Phrynocephalus mystaceus/p_mystaceus/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C9BA0E7E-D880-DD44-AB23-2DBAFE90E853}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14680" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14540" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorted" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <sheet name="graphs_noose" sheetId="9" r:id="rId9"/>
     <sheet name="graph_birdfield" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,18 +37,18 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Martin Whiting</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -56,12 +57,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Yes/No if lizard extended flaps during capture (noosing/handling). Lizard tapped ten times on snout if it didn't flare during capture.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yes/No if lizard extended flaps during capture (noosing/handling). Lizard tapped ten times on snout if it didn't flare during capture.</t>
         </r>
       </text>
     </comment>
@@ -70,12 +80,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Martin Whiting</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -658,8 +668,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -703,8 +713,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,6 +737,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +843,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -838,6 +873,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -925,6 +963,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1251,7 +1292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2824,7 +2865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2909,7 +2950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -3529,7 +3570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3951,7 +3992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4411,7 +4452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4870,12 +4911,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40:E41"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4910,7 +4951,7 @@
       <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -4927,7 +4968,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -4944,7 +4985,7 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -4961,7 +5002,7 @@
       <c r="C5" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4975,7 +5016,7 @@
       <c r="C6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -4992,7 +5033,7 @@
       <c r="C7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -5009,7 +5050,7 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -5026,7 +5067,7 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -5043,7 +5084,7 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -5060,7 +5101,7 @@
       <c r="C11" t="s">
         <v>112</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -5077,7 +5118,7 @@
       <c r="C12" t="s">
         <v>115</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -5094,7 +5135,7 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -5111,7 +5152,7 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -5128,7 +5169,7 @@
       <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -5145,7 +5186,7 @@
       <c r="C16" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5159,7 +5200,7 @@
       <c r="C17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -5176,7 +5217,7 @@
       <c r="C18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -5193,7 +5234,7 @@
       <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -5210,7 +5251,7 @@
       <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -5227,7 +5268,7 @@
       <c r="C21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -5244,7 +5285,7 @@
       <c r="C22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -5261,7 +5302,7 @@
       <c r="C23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -5278,7 +5319,7 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -5295,7 +5336,7 @@
       <c r="C25" t="s">
         <v>11</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -5312,7 +5353,7 @@
       <c r="C26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -5329,7 +5370,7 @@
       <c r="C27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -5346,7 +5387,7 @@
       <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -5363,7 +5404,7 @@
       <c r="C29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -5380,7 +5421,7 @@
       <c r="C30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -5397,7 +5438,7 @@
       <c r="C31" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5492,10 +5533,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
@@ -6604,7 +6645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6716,7 +6757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>